<commit_message>
Update aerodynamic design spreadsheet
Modified ESTYCTRL HRD-02 spreadsheet with changes to aerodynamic and dynamic design data. Review for updated calculations or input values.
</commit_message>
<xml_diff>
--- a/ESTYCTRL HRD-02 Diseño Aerodinámico y dinámico Rev.1 (1).xlsx
+++ b/ESTYCTRL HRD-02 Diseño Aerodinámico y dinámico Rev.1 (1).xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonardo.valadez\Documents\Repositorios\Recovery-systems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonardo.valadez\Documents\00 Repos\rocketry-aero-and-stability\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3842,18 +3842,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3863,25 +3851,58 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3897,15 +3918,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3932,22 +3944,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4291,11 +4291,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1322025648"/>
-        <c:axId val="-1322019664"/>
+        <c:axId val="340953304"/>
+        <c:axId val="340959968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1322025648"/>
+        <c:axId val="340953304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4423,14 +4423,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1322019664"/>
+        <c:crossAx val="340959968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.30000000000000004"/>
         <c:minorUnit val="0.30000000000000004"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1322019664"/>
+        <c:axId val="340959968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4604,7 +4604,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1322025648"/>
+        <c:crossAx val="340953304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
@@ -4794,11 +4794,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1205955648"/>
-        <c:axId val="-1205960000"/>
+        <c:axId val="342803960"/>
+        <c:axId val="342799648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1205955648"/>
+        <c:axId val="342803960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4869,12 +4869,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1205960000"/>
+        <c:crossAx val="342799648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1205960000"/>
+        <c:axId val="342799648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4945,7 +4945,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1205955648"/>
+        <c:crossAx val="342803960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6108,11 +6108,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1205958912"/>
-        <c:axId val="-1205957824"/>
+        <c:axId val="342804744"/>
+        <c:axId val="339079808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1205958912"/>
+        <c:axId val="342804744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6238,12 +6238,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1205957824"/>
+        <c:crossAx val="339079808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1205957824"/>
+        <c:axId val="339079808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6369,7 +6369,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1205958912"/>
+        <c:crossAx val="342804744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7469,11 +7469,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1205957280"/>
-        <c:axId val="-1205955104"/>
+        <c:axId val="339077848"/>
+        <c:axId val="339080592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1205957280"/>
+        <c:axId val="339077848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7599,12 +7599,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1205955104"/>
+        <c:crossAx val="339080592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1205955104"/>
+        <c:axId val="339080592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7730,7 +7730,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1205957280"/>
+        <c:crossAx val="339077848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7992,11 +7992,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1205952928"/>
-        <c:axId val="-1205956736"/>
+        <c:axId val="339073144"/>
+        <c:axId val="339078240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1205952928"/>
+        <c:axId val="339073144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8108,12 +8108,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1205956736"/>
+        <c:crossAx val="339078240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1205956736"/>
+        <c:axId val="339078240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -8226,7 +8226,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1205952928"/>
+        <c:crossAx val="339073144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8451,11 +8451,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1200708192"/>
-        <c:axId val="-1200706560"/>
+        <c:axId val="339076280"/>
+        <c:axId val="339078632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1200708192"/>
+        <c:axId val="339076280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8512,12 +8512,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1200706560"/>
+        <c:crossAx val="339078632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1200706560"/>
+        <c:axId val="339078632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8574,7 +8574,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1200708192"/>
+        <c:crossAx val="339076280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8799,11 +8799,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1200713632"/>
-        <c:axId val="-1200709824"/>
+        <c:axId val="339079024"/>
+        <c:axId val="339074320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1200713632"/>
+        <c:axId val="339079024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8860,12 +8860,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1200709824"/>
+        <c:crossAx val="339074320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1200709824"/>
+        <c:axId val="339074320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -8923,7 +8923,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1200713632"/>
+        <c:crossAx val="339079024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9837,11 +9837,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1200707648"/>
-        <c:axId val="-1200712544"/>
+        <c:axId val="339079416"/>
+        <c:axId val="339075496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1200707648"/>
+        <c:axId val="339079416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9898,12 +9898,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1200712544"/>
+        <c:crossAx val="339075496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1200712544"/>
+        <c:axId val="339075496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2"/>
@@ -9961,7 +9961,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1200707648"/>
+        <c:crossAx val="339079416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10403,11 +10403,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1200708736"/>
-        <c:axId val="-1200707104"/>
+        <c:axId val="339075104"/>
+        <c:axId val="339075888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1200708736"/>
+        <c:axId val="339075104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10464,12 +10464,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1200707104"/>
+        <c:crossAx val="339075888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1200707104"/>
+        <c:axId val="339075888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10526,7 +10526,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1200708736"/>
+        <c:crossAx val="339075104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10736,8 +10736,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1200712000"/>
-        <c:axId val="-1200713088"/>
+        <c:axId val="346218776"/>
+        <c:axId val="346225048"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -10845,11 +10845,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1200711456"/>
-        <c:axId val="-1200709280"/>
+        <c:axId val="346221520"/>
+        <c:axId val="346219168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1200712000"/>
+        <c:axId val="346218776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10906,7 +10906,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1200713088"/>
+        <c:crossAx val="346225048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10914,7 +10914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1200713088"/>
+        <c:axId val="346225048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10971,12 +10971,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1200712000"/>
+        <c:crossAx val="346218776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1200709280"/>
+        <c:axId val="346219168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11019,12 +11019,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1200711456"/>
+        <c:crossAx val="346221520"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1200711456"/>
+        <c:axId val="346221520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11034,7 +11034,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1200709280"/>
+        <c:crossAx val="346219168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11321,11 +11321,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1200710912"/>
-        <c:axId val="-1200710368"/>
+        <c:axId val="346220736"/>
+        <c:axId val="346223872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1200710912"/>
+        <c:axId val="346220736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -11383,12 +11383,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1200710368"/>
+        <c:crossAx val="346223872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1200710368"/>
+        <c:axId val="346223872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11445,7 +11445,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1200710912"/>
+        <c:crossAx val="346220736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11930,11 +11930,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1322022384"/>
-        <c:axId val="-1322018576"/>
+        <c:axId val="340959576"/>
+        <c:axId val="340954480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1322022384"/>
+        <c:axId val="340959576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12002,12 +12002,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1322018576"/>
+        <c:crossAx val="340954480"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1322018576"/>
+        <c:axId val="340954480"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -12078,7 +12078,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1322022384"/>
+        <c:crossAx val="340959576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12474,11 +12474,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1322019120"/>
-        <c:axId val="-1322018032"/>
+        <c:axId val="340958008"/>
+        <c:axId val="340953696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1322019120"/>
+        <c:axId val="340958008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12549,12 +12549,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1322018032"/>
+        <c:crossAx val="340953696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1322018032"/>
+        <c:axId val="340953696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12625,7 +12625,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1322019120"/>
+        <c:crossAx val="340958008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12935,11 +12935,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1322015312"/>
-        <c:axId val="-1322014768"/>
+        <c:axId val="340957616"/>
+        <c:axId val="339454472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1322015312"/>
+        <c:axId val="340957616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13009,12 +13009,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1322014768"/>
+        <c:crossAx val="339454472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1322014768"/>
+        <c:axId val="339454472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13085,7 +13085,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1322015312"/>
+        <c:crossAx val="340957616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13271,11 +13271,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1322014224"/>
-        <c:axId val="-1538164992"/>
+        <c:axId val="342806312"/>
+        <c:axId val="342805136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1322014224"/>
+        <c:axId val="342806312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13346,12 +13346,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1538164992"/>
+        <c:crossAx val="342805136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1538164992"/>
+        <c:axId val="342805136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8"/>
@@ -13423,7 +13423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1322014224"/>
+        <c:crossAx val="342806312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14343,11 +14343,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1538170976"/>
-        <c:axId val="-1538174784"/>
+        <c:axId val="342800824"/>
+        <c:axId val="342805920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1538170976"/>
+        <c:axId val="342800824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14418,12 +14418,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1538174784"/>
+        <c:crossAx val="342805920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1538174784"/>
+        <c:axId val="342805920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14494,7 +14494,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1538170976"/>
+        <c:crossAx val="342800824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14683,8 +14683,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1205959456"/>
-        <c:axId val="-1205958368"/>
+        <c:axId val="342800432"/>
+        <c:axId val="342798864"/>
         <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -14810,7 +14810,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1205959456"/>
+        <c:axId val="342800432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -14882,12 +14882,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1205958368"/>
+        <c:crossAx val="342798864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1205958368"/>
+        <c:axId val="342798864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14958,7 +14958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1205959456"/>
+        <c:crossAx val="342800432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15144,11 +15144,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1205954016"/>
-        <c:axId val="-1205954560"/>
+        <c:axId val="342801216"/>
+        <c:axId val="342802784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1205954016"/>
+        <c:axId val="342801216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15219,12 +15219,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1205954560"/>
+        <c:crossAx val="342802784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1205954560"/>
+        <c:axId val="342802784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8"/>
@@ -15296,7 +15296,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1205954016"/>
+        <c:crossAx val="342801216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15485,11 +15485,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1205953472"/>
-        <c:axId val="-1205956192"/>
+        <c:axId val="342802000"/>
+        <c:axId val="342803176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1205953472"/>
+        <c:axId val="342802000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15560,12 +15560,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1205956192"/>
+        <c:crossAx val="342803176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1205956192"/>
+        <c:axId val="342803176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15636,7 +15636,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1205953472"/>
+        <c:crossAx val="342802000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -25965,7 +25965,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{393B3C67-1ABC-2789-344B-126A3B5F8F18}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393B3C67-1ABC-2789-344B-126A3B5F8F18}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26022,7 +26022,7 @@
             <xdr:cNvPr id="11" name="TextBox 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{37A524B4-13F7-A024-0584-ED9E880D868F}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37A524B4-13F7-A024-0584-ED9E880D868F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -26363,10 +26363,10 @@
         <xdr:cNvPr id="12" name="Chart 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8696CF88-4D17-58E0-4547-0F4FEA49BBCA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8696CF88-4D17-58E0-4547-0F4FEA49BBCA}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{37A524B4-13F7-A024-0584-ED9E880D868F}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{37A524B4-13F7-A024-0584-ED9E880D868F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26399,7 +26399,7 @@
             <xdr:cNvPr id="13" name="TextBox 12">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F27C3274-15D1-951A-7FD8-DA1BEAC20F75}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F27C3274-15D1-951A-7FD8-DA1BEAC20F75}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -26631,7 +26631,7 @@
             <xdr:cNvPr id="14" name="TextBox 13">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5AE2CABF-230F-1FCE-16A4-CED18BDBB96F}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AE2CABF-230F-1FCE-16A4-CED18BDBB96F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -26865,7 +26865,7 @@
             <xdr:cNvPr id="15" name="TextBox 14">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8015B4A1-1918-BE89-980C-B85DE46BD6BC}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8015B4A1-1918-BE89-980C-B85DE46BD6BC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -27150,7 +27150,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{25F80604-448F-B015-D105-A97A13CB0066}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25F80604-448F-B015-D105-A97A13CB0066}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27224,7 +27224,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B846C0C-F558-AFB6-E24C-A1AB278BB42E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B846C0C-F558-AFB6-E24C-A1AB278BB42E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -27295,7 +27295,7 @@
             <xdr:cNvPr id="5" name="TextBox 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A8BA3FBC-9103-9850-09A8-DDCD8887D004}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8BA3FBC-9103-9850-09A8-DDCD8887D004}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -27680,7 +27680,7 @@
             <xdr:cNvPr id="6" name="TextBox 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B7E12D9-9242-9E1C-099C-D2BBD2CCD9CB}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B7E12D9-9242-9E1C-099C-D2BBD2CCD9CB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -28175,10 +28175,10 @@
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{10EB7F2F-3037-0F02-65F4-9470FC24037D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10EB7F2F-3037-0F02-65F4-9470FC24037D}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{4B7E12D9-9242-9E1C-099C-D2BBD2CCD9CB}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4B7E12D9-9242-9E1C-099C-D2BBD2CCD9CB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28214,10 +28214,10 @@
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1E1B4768-DDEF-37F2-E2F6-DF6922649F41}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E1B4768-DDEF-37F2-E2F6-DF6922649F41}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{10EB7F2F-3037-0F02-65F4-9470FC24037D}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{10EB7F2F-3037-0F02-65F4-9470FC24037D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28258,7 +28258,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1C3C2806-C192-4C8E-400B-77250FF88002}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C3C2806-C192-4C8E-400B-77250FF88002}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28302,7 +28302,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1E49E023-F1F9-85DB-71B0-14903EA1E2E8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E49E023-F1F9-85DB-71B0-14903EA1E2E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28346,7 +28346,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{31466A9B-9FE0-4282-E083-96028C27B7F0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31466A9B-9FE0-4282-E083-96028C27B7F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28395,7 +28395,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AF0E0E67-9C36-058A-4D85-04C0B1DFFA5C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF0E0E67-9C36-058A-4D85-04C0B1DFFA5C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28431,10 +28431,10 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E128D49A-3629-4BBF-9581-DB9D69B8A541}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E128D49A-3629-4BBF-9581-DB9D69B8A541}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{AF0E0E67-9C36-058A-4D85-04C0B1DFFA5C}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{AF0E0E67-9C36-058A-4D85-04C0B1DFFA5C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28472,10 +28472,10 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4705D049-9711-4AD6-8388-EAF961A55C4C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4705D049-9711-4AD6-8388-EAF961A55C4C}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{E128D49A-3629-4BBF-9581-DB9D69B8A541}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E128D49A-3629-4BBF-9581-DB9D69B8A541}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28513,10 +28513,10 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{64CC32F9-70E7-407E-A2B4-7366728088AD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64CC32F9-70E7-407E-A2B4-7366728088AD}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{4705D049-9711-4AD6-8388-EAF961A55C4C}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4705D049-9711-4AD6-8388-EAF961A55C4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28554,10 +28554,10 @@
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{250CC376-444D-4A69-B396-08361C76F808}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{250CC376-444D-4A69-B396-08361C76F808}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{64CC32F9-70E7-407E-A2B4-7366728088AD}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{64CC32F9-70E7-407E-A2B4-7366728088AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28595,10 +28595,10 @@
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C15CA873-26E1-4AC6-B585-4EB97F3C73DC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C15CA873-26E1-4AC6-B585-4EB97F3C73DC}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{250CC376-444D-4A69-B396-08361C76F808}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{250CC376-444D-4A69-B396-08361C76F808}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28636,10 +28636,10 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9A60D0BB-D2DB-4D29-AC4E-706AD0B20703}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A60D0BB-D2DB-4D29-AC4E-706AD0B20703}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{C15CA873-26E1-4AC6-B585-4EB97F3C73DC}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{C15CA873-26E1-4AC6-B585-4EB97F3C73DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28672,7 +28672,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6F2E01F0-7A94-06DF-7AB3-CD6A31C3FE8D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F2E01F0-7A94-06DF-7AB3-CD6A31C3FE8D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -28729,7 +28729,7 @@
             <xdr:cNvPr id="10" name="TextBox 9">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{120D1765-6CE0-A43C-C2C3-6C5CED27D83A}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{120D1765-6CE0-A43C-C2C3-6C5CED27D83A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -29002,7 +29002,7 @@
             <xdr:cNvPr id="12" name="TextBox 11">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7BB379C5-A5E3-077C-7C48-41207301E333}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BB379C5-A5E3-077C-7C48-41207301E333}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -29351,7 +29351,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E3C537F2-31BC-477B-A2BA-3324E8A581D6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3C537F2-31BC-477B-A2BA-3324E8A581D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29389,10 +29389,10 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E18AE237-AB9B-443B-9AC6-0A486D849990}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E18AE237-AB9B-443B-9AC6-0A486D849990}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" pred="{E3C537F2-31BC-477B-A2BA-3324E8A581D6}"/>
+              <a16:predDERef xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E3C537F2-31BC-477B-A2BA-3324E8A581D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29430,10 +29430,10 @@
         <xdr:cNvPr id="5" name="Rectangle: Rounded Corners 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D877167B-41EB-4438-B309-3687EC1249E9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D877167B-41EB-4438-B309-3687EC1249E9}"/>
             </a:ext>
             <a:ext uri="{6ECC49D1-AA05-4338-93AA-15A1B29DFB0A}">
-              <asl:scriptLink xmlns:asl="http://schemas.microsoft.com/office/drawing/2021/scriptlink" xmlns="" val="{&quot;shareId&quot;:&quot;ms-officescript%3A%2F%2Fonedrive_business_sharinglink%2Fu!aHR0cHM6Ly91YW5sZWR1LW15LnNoYXJlcG9pbnQuY29tLzp1Oi9nL3BlcnNvbmFsL2p1YW5fdmFsYWRlem9fdWFubF9lZHVfbXgvRWZvVnBMM2VtV3RPbzlUVTRvVUlHQmNCRlJyQnlnX2V0OW1LWVd3VTNFU3NaUQ&quot;}"/>
+              <asl:scriptLink xmlns="" xmlns:asl="http://schemas.microsoft.com/office/drawing/2021/scriptlink" val="{&quot;shareId&quot;:&quot;ms-officescript%3A%2F%2Fonedrive_business_sharinglink%2Fu!aHR0cHM6Ly91YW5sZWR1LW15LnNoYXJlcG9pbnQuY29tLzp1Oi9nL3BlcnNvbmFsL2p1YW5fdmFsYWRlem9fdWFubF9lZHVfbXgvRWZvVnBMM2VtV3RPbzlUVTRvVUlHQmNCRlJyQnlnX2V0OW1LWVd3VTNFU3NaUQ&quot;}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29514,7 +29514,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E58467C2-2019-BCCC-3B09-5F212FBC35F6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E58467C2-2019-BCCC-3B09-5F212FBC35F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29563,7 +29563,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29599,7 +29599,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29635,7 +29635,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -29668,14 +29668,14 @@
       <xdr:rowOff>38954</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1482329" cy="315792"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6D022E62-4A35-4DCD-8D2A-B3B77A9519EE}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D022E62-4A35-4DCD-8D2A-B3B77A9519EE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -29907,7 +29907,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -29972,14 +29972,14 @@
       <xdr:rowOff>81643</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1118063" cy="315792"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{498D211D-116C-4881-B0FD-4DE2CAB102D0}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{498D211D-116C-4881-B0FD-4DE2CAB102D0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -30111,7 +30111,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -30186,7 +30186,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EDE16BEB-BF7B-48BC-A264-C6EB2A678B38}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDE16BEB-BF7B-48BC-A264-C6EB2A678B38}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30235,7 +30235,7 @@
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{940D527C-4366-00CE-4B25-D1D345FA8B13}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{940D527C-4366-00CE-4B25-D1D345FA8B13}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30268,7 +30268,7 @@
             <xdr:cNvPr id="10" name="TextBox 9">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A761C379-9697-216A-9A7E-CFB8449EE35F}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A761C379-9697-216A-9A7E-CFB8449EE35F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -30513,7 +30513,7 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9C9DD64C-8DAF-E3DC-52EF-344D71B514CD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C9DD64C-8DAF-E3DC-52EF-344D71B514CD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -30546,7 +30546,7 @@
             <xdr:cNvPr id="12" name="TextBox 11">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C30842E1-FA76-C7DF-5357-28BDD94979CA}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C30842E1-FA76-C7DF-5357-28BDD94979CA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -30932,7 +30932,7 @@
             <xdr:cNvPr id="13" name="TextBox 12">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{238526A6-FCD4-8548-FF55-6B3C91F39C4B}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{238526A6-FCD4-8548-FF55-6B3C91F39C4B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -31317,7 +31317,7 @@
             <xdr:cNvPr id="14" name="TextBox 13">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1D924C9F-B1DD-4B9D-BFCF-B5695F959620}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D924C9F-B1DD-4B9D-BFCF-B5695F959620}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -31678,7 +31678,7 @@
         <xdr:cNvPr id="15" name="Chart 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00593C10-B837-4C24-7607-B834AEF6849E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00593C10-B837-4C24-7607-B834AEF6849E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31714,7 +31714,7 @@
         <xdr:cNvPr id="16" name="Chart 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{064315BC-E7A3-C5F1-199F-03D3DC0B7A7C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{064315BC-E7A3-C5F1-199F-03D3DC0B7A7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31747,7 +31747,7 @@
             <xdr:cNvPr id="17" name="TextBox 16">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8CDE8A02-B0ED-012D-019B-E87D218D6924}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CDE8A02-B0ED-012D-019B-E87D218D6924}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -32094,7 +32094,7 @@
             <xdr:cNvPr id="18" name="TextBox 17">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE797A0D-38FE-68C2-1937-5CEA76EEAF0D}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE797A0D-38FE-68C2-1937-5CEA76EEAF0D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -32490,7 +32490,7 @@
             <xdr:cNvPr id="19" name="TextBox 18">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6623A625-4973-241C-C2D8-E55AF8EEB25E}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6623A625-4973-241C-C2D8-E55AF8EEB25E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -32746,7 +32746,7 @@
             <xdr:cNvPr id="2" name="TextBox 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2736D442-88E4-B09D-E012-92D915CB7DF1}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2736D442-88E4-B09D-E012-92D915CB7DF1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -33052,7 +33052,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1EA6BB45-C842-F85B-2CD2-48F390F79360}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EA6BB45-C842-F85B-2CD2-48F390F79360}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33096,7 +33096,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{71695D33-2EF6-CC71-803C-53E251A3DCB2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71695D33-2EF6-CC71-803C-53E251A3DCB2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33137,7 +33137,7 @@
             <xdr:cNvPr id="5" name="TextBox 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F9B0840E-4CE9-ABAA-F86E-A2C5A3298F58}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9B0840E-4CE9-ABAA-F86E-A2C5A3298F58}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -33365,7 +33365,7 @@
             <xdr:cNvPr id="6" name="TextBox 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{26F5E52C-9462-4017-812B-1B440BA856B0}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26F5E52C-9462-4017-812B-1B440BA856B0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -33611,7 +33611,7 @@
             <xdr:cNvPr id="7" name="TextBox 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EDCB27B8-A82C-0368-52DC-5AD97013AFC5}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDCB27B8-A82C-0368-52DC-5AD97013AFC5}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -33817,7 +33817,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A4E79A02-8F63-33C0-1D45-29D3BDA633AD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4E79A02-8F63-33C0-1D45-29D3BDA633AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33866,7 +33866,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FDD733D0-702B-9D6D-B7A4-AE79237D48AA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDD733D0-702B-9D6D-B7A4-AE79237D48AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -33907,7 +33907,7 @@
             <xdr:cNvPr id="3" name="TextBox 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2D898092-0340-1DEC-094C-4073F2FA1F95}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D898092-0340-1DEC-094C-4073F2FA1F95}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -34110,7 +34110,7 @@
             <xdr:cNvPr id="4" name="TextBox 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000004000000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -34301,7 +34301,7 @@
             <xdr:cNvPr id="5" name="TextBox 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000005000000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -34486,7 +34486,7 @@
             <xdr:cNvPr id="6" name="TextBox 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2D898092-0340-1DEC-094C-4073F2FA1F95}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D898092-0340-1DEC-094C-4073F2FA1F95}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -34722,7 +34722,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FDD733D0-702B-9D6D-B7A4-AE79237D48AA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDD733D0-702B-9D6D-B7A4-AE79237D48AA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -34763,7 +34763,7 @@
             <xdr:cNvPr id="2" name="TextBox 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2D898092-0340-1DEC-094C-4073F2FA1F95}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D898092-0340-1DEC-094C-4073F2FA1F95}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -34966,7 +34966,7 @@
             <xdr:cNvPr id="3" name="TextBox 2">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000003000000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000003000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -35156,7 +35156,7 @@
             <xdr:cNvPr id="4" name="TextBox 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -35340,7 +35340,7 @@
             <xdr:cNvPr id="6" name="TextBox 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2D898092-0340-1DEC-094C-4073F2FA1F95}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D898092-0340-1DEC-094C-4073F2FA1F95}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -42600,10 +42600,10 @@
   <sheetData>
     <row r="1" spans="2:22" ht="15" thickBot="1"/>
     <row r="2" spans="2:22" ht="37.15" customHeight="1">
-      <c r="B2" s="330" t="s">
+      <c r="B2" s="348" t="s">
         <v>182</v>
       </c>
-      <c r="C2" s="331"/>
+      <c r="C2" s="350"/>
     </row>
     <row r="3" spans="2:22">
       <c r="B3" s="3" t="s">
@@ -42673,13 +42673,13 @@
       <c r="B12" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C12" s="334" t="s">
+      <c r="C12" s="330" t="s">
         <v>185</v>
       </c>
-      <c r="D12" s="335"/>
-      <c r="E12" s="335"/>
-      <c r="F12" s="335"/>
-      <c r="G12" s="336"/>
+      <c r="D12" s="331"/>
+      <c r="E12" s="331"/>
+      <c r="F12" s="331"/>
+      <c r="G12" s="332"/>
       <c r="H12" s="1" t="s">
         <v>186</v>
       </c>
@@ -42694,13 +42694,13 @@
       <c r="N12" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="O12" s="334" t="s">
+      <c r="O12" s="330" t="s">
         <v>189</v>
       </c>
-      <c r="P12" s="335"/>
-      <c r="Q12" s="335"/>
-      <c r="R12" s="335"/>
-      <c r="S12" s="336"/>
+      <c r="P12" s="331"/>
+      <c r="Q12" s="331"/>
+      <c r="R12" s="331"/>
+      <c r="S12" s="332"/>
       <c r="T12" s="1" t="s">
         <v>186</v>
       </c>
@@ -42712,7 +42712,7 @@
       </c>
     </row>
     <row r="13" spans="2:22">
-      <c r="B13" s="332" t="s">
+      <c r="B13" s="345" t="s">
         <v>190</v>
       </c>
       <c r="C13" s="71"/>
@@ -42732,7 +42732,7 @@
       </c>
       <c r="L13" s="64"/>
       <c r="M13" s="64"/>
-      <c r="N13" s="332" t="s">
+      <c r="N13" s="345" t="s">
         <v>190</v>
       </c>
       <c r="O13" s="71"/>
@@ -42752,7 +42752,7 @@
       </c>
     </row>
     <row r="14" spans="2:22">
-      <c r="B14" s="333"/>
+      <c r="B14" s="346"/>
       <c r="C14" s="74"/>
       <c r="D14" s="64"/>
       <c r="E14" s="64"/>
@@ -42772,7 +42772,7 @@
       </c>
       <c r="L14" s="64"/>
       <c r="M14" s="64"/>
-      <c r="N14" s="333"/>
+      <c r="N14" s="346"/>
       <c r="O14" s="74"/>
       <c r="P14" s="64"/>
       <c r="Q14" s="64"/>
@@ -42792,7 +42792,7 @@
       </c>
     </row>
     <row r="15" spans="2:22">
-      <c r="B15" s="333"/>
+      <c r="B15" s="346"/>
       <c r="C15" s="74"/>
       <c r="D15" s="64"/>
       <c r="E15" s="64"/>
@@ -42812,7 +42812,7 @@
       </c>
       <c r="L15" s="64"/>
       <c r="M15" s="64"/>
-      <c r="N15" s="333"/>
+      <c r="N15" s="346"/>
       <c r="O15" s="74"/>
       <c r="P15" s="64"/>
       <c r="Q15" s="64"/>
@@ -42832,7 +42832,7 @@
       </c>
     </row>
     <row r="16" spans="2:22">
-      <c r="B16" s="333"/>
+      <c r="B16" s="346"/>
       <c r="C16" s="74"/>
       <c r="D16" s="64"/>
       <c r="E16" s="64"/>
@@ -42852,7 +42852,7 @@
       </c>
       <c r="L16" s="64"/>
       <c r="M16" s="64"/>
-      <c r="N16" s="333"/>
+      <c r="N16" s="346"/>
       <c r="O16" s="74"/>
       <c r="P16" s="64"/>
       <c r="Q16" s="64"/>
@@ -42872,7 +42872,7 @@
       </c>
     </row>
     <row r="17" spans="2:22">
-      <c r="B17" s="333"/>
+      <c r="B17" s="346"/>
       <c r="C17" s="74"/>
       <c r="D17" s="64"/>
       <c r="E17" s="64"/>
@@ -42892,7 +42892,7 @@
       </c>
       <c r="L17" s="64"/>
       <c r="M17" s="64"/>
-      <c r="N17" s="333"/>
+      <c r="N17" s="346"/>
       <c r="O17" s="74"/>
       <c r="P17" s="64"/>
       <c r="Q17" s="64"/>
@@ -42912,7 +42912,7 @@
       </c>
     </row>
     <row r="18" spans="2:22">
-      <c r="B18" s="333"/>
+      <c r="B18" s="346"/>
       <c r="C18" s="74"/>
       <c r="D18" s="64"/>
       <c r="E18" s="64"/>
@@ -42932,7 +42932,7 @@
       </c>
       <c r="L18" s="64"/>
       <c r="M18" s="64"/>
-      <c r="N18" s="333"/>
+      <c r="N18" s="346"/>
       <c r="O18" s="74"/>
       <c r="P18" s="64"/>
       <c r="Q18" s="64"/>
@@ -42952,7 +42952,7 @@
       </c>
     </row>
     <row r="19" spans="2:22">
-      <c r="B19" s="333"/>
+      <c r="B19" s="346"/>
       <c r="C19" s="74"/>
       <c r="D19" s="64"/>
       <c r="E19" s="64"/>
@@ -42972,7 +42972,7 @@
       </c>
       <c r="L19" s="64"/>
       <c r="M19" s="64"/>
-      <c r="N19" s="333"/>
+      <c r="N19" s="346"/>
       <c r="O19" s="74"/>
       <c r="P19" s="64"/>
       <c r="Q19" s="64"/>
@@ -42992,7 +42992,7 @@
       </c>
     </row>
     <row r="20" spans="2:22">
-      <c r="B20" s="333"/>
+      <c r="B20" s="346"/>
       <c r="C20" s="74"/>
       <c r="D20" s="64"/>
       <c r="E20" s="64"/>
@@ -43012,7 +43012,7 @@
       </c>
       <c r="L20" s="64"/>
       <c r="M20" s="64"/>
-      <c r="N20" s="333"/>
+      <c r="N20" s="346"/>
       <c r="O20" s="74"/>
       <c r="P20" s="64"/>
       <c r="Q20" s="64"/>
@@ -43032,7 +43032,7 @@
       </c>
     </row>
     <row r="21" spans="2:22">
-      <c r="B21" s="333"/>
+      <c r="B21" s="346"/>
       <c r="C21" s="74"/>
       <c r="D21" s="64"/>
       <c r="E21" s="64"/>
@@ -43052,7 +43052,7 @@
       </c>
       <c r="L21" s="64"/>
       <c r="M21" s="64"/>
-      <c r="N21" s="333"/>
+      <c r="N21" s="346"/>
       <c r="O21" s="74"/>
       <c r="P21" s="64"/>
       <c r="Q21" s="64"/>
@@ -43072,7 +43072,7 @@
       </c>
     </row>
     <row r="22" spans="2:22" ht="15" thickBot="1">
-      <c r="B22" s="333"/>
+      <c r="B22" s="346"/>
       <c r="C22" s="74"/>
       <c r="D22" s="64"/>
       <c r="E22" s="64"/>
@@ -43092,7 +43092,7 @@
       </c>
       <c r="L22" s="64"/>
       <c r="M22" s="64"/>
-      <c r="N22" s="337"/>
+      <c r="N22" s="347"/>
       <c r="O22" s="74"/>
       <c r="P22" s="64"/>
       <c r="Q22" s="64"/>
@@ -43112,7 +43112,7 @@
       </c>
     </row>
     <row r="23" spans="2:22" ht="14.45" customHeight="1">
-      <c r="B23" s="341" t="s">
+      <c r="B23" s="365" t="s">
         <v>191</v>
       </c>
       <c r="C23" s="66"/>
@@ -43122,8 +43122,8 @@
       <c r="E23" s="65"/>
       <c r="F23" s="65"/>
       <c r="G23" s="65"/>
-      <c r="K23" s="339"/>
-      <c r="N23" s="340" t="s">
+      <c r="K23" s="343"/>
+      <c r="N23" s="364" t="s">
         <v>191</v>
       </c>
       <c r="O23" s="66" t="s">
@@ -43138,7 +43138,7 @@
       <c r="S23" s="65"/>
     </row>
     <row r="24" spans="2:22">
-      <c r="B24" s="341"/>
+      <c r="B24" s="365"/>
       <c r="C24" s="67" t="s">
         <v>193</v>
       </c>
@@ -43146,8 +43146,8 @@
         <f>(F25/2)/(F26)</f>
         <v>0.13333333333333333</v>
       </c>
-      <c r="K24" s="339"/>
-      <c r="N24" s="341"/>
+      <c r="K24" s="343"/>
+      <c r="N24" s="365"/>
       <c r="O24" s="67" t="s">
         <v>193</v>
       </c>
@@ -43156,7 +43156,7 @@
       </c>
     </row>
     <row r="25" spans="2:22">
-      <c r="B25" s="341"/>
+      <c r="B25" s="365"/>
       <c r="C25" s="67" t="s">
         <v>195</v>
       </c>
@@ -43174,8 +43174,8 @@
       <c r="G25" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="K25" s="339"/>
-      <c r="N25" s="341"/>
+      <c r="K25" s="343"/>
+      <c r="N25" s="365"/>
       <c r="O25" s="67" t="s">
         <v>195</v>
       </c>
@@ -43195,7 +43195,7 @@
       </c>
     </row>
     <row r="26" spans="2:22" ht="14.45" customHeight="1">
-      <c r="B26" s="341"/>
+      <c r="B26" s="365"/>
       <c r="C26" s="68" t="s">
         <v>198</v>
       </c>
@@ -43212,8 +43212,8 @@
       <c r="G26" s="69" t="s">
         <v>197</v>
       </c>
-      <c r="K26" s="339"/>
-      <c r="N26" s="341"/>
+      <c r="K26" s="343"/>
+      <c r="N26" s="365"/>
       <c r="O26" s="68" t="s">
         <v>198</v>
       </c>
@@ -43235,25 +43235,25 @@
       <c r="B27" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C27" s="342" t="s">
+      <c r="C27" s="333" t="s">
         <v>200</v>
       </c>
-      <c r="D27" s="342"/>
-      <c r="E27" s="342"/>
-      <c r="F27" s="342"/>
-      <c r="G27" s="342"/>
+      <c r="D27" s="333"/>
+      <c r="E27" s="333"/>
+      <c r="F27" s="333"/>
+      <c r="G27" s="333"/>
       <c r="L27" s="64"/>
       <c r="M27" s="64"/>
       <c r="N27" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="O27" s="342" t="s">
+      <c r="O27" s="333" t="s">
         <v>200</v>
       </c>
-      <c r="P27" s="342"/>
-      <c r="Q27" s="342"/>
-      <c r="R27" s="342"/>
-      <c r="S27" s="342"/>
+      <c r="P27" s="333"/>
+      <c r="Q27" s="333"/>
+      <c r="R27" s="333"/>
+      <c r="S27" s="333"/>
     </row>
     <row r="28" spans="2:22" ht="57">
       <c r="B28" s="2" t="s">
@@ -43295,14 +43295,14 @@
       </c>
     </row>
     <row r="31" spans="2:22">
-      <c r="B31" s="332" t="s">
+      <c r="B31" s="345" t="s">
         <v>203</v>
       </c>
-      <c r="C31" s="330"/>
-      <c r="D31" s="343"/>
-      <c r="E31" s="343"/>
-      <c r="F31" s="343"/>
-      <c r="G31" s="331"/>
+      <c r="C31" s="348"/>
+      <c r="D31" s="349"/>
+      <c r="E31" s="349"/>
+      <c r="F31" s="349"/>
+      <c r="G31" s="350"/>
       <c r="H31" s="1">
         <f>H22</f>
         <v>30</v>
@@ -43317,12 +43317,12 @@
       </c>
     </row>
     <row r="32" spans="2:22">
-      <c r="B32" s="333"/>
-      <c r="C32" s="344"/>
-      <c r="D32" s="338"/>
-      <c r="E32" s="338"/>
-      <c r="F32" s="338"/>
-      <c r="G32" s="345"/>
+      <c r="B32" s="346"/>
+      <c r="C32" s="351"/>
+      <c r="D32" s="340"/>
+      <c r="E32" s="340"/>
+      <c r="F32" s="340"/>
+      <c r="G32" s="352"/>
       <c r="H32" s="12">
         <f>(D43/8/2)+H31</f>
         <v>36.25</v>
@@ -43337,12 +43337,12 @@
       </c>
     </row>
     <row r="33" spans="2:24">
-      <c r="B33" s="333"/>
-      <c r="C33" s="344"/>
-      <c r="D33" s="338"/>
-      <c r="E33" s="338"/>
-      <c r="F33" s="338"/>
-      <c r="G33" s="345"/>
+      <c r="B33" s="346"/>
+      <c r="C33" s="351"/>
+      <c r="D33" s="340"/>
+      <c r="E33" s="340"/>
+      <c r="F33" s="340"/>
+      <c r="G33" s="352"/>
       <c r="H33" s="12">
         <f>($D$43/8/2)*2+(H32)</f>
         <v>48.75</v>
@@ -43357,12 +43357,12 @@
       </c>
     </row>
     <row r="34" spans="2:24">
-      <c r="B34" s="333"/>
-      <c r="C34" s="344"/>
-      <c r="D34" s="338"/>
-      <c r="E34" s="338"/>
-      <c r="F34" s="338"/>
-      <c r="G34" s="345"/>
+      <c r="B34" s="346"/>
+      <c r="C34" s="351"/>
+      <c r="D34" s="340"/>
+      <c r="E34" s="340"/>
+      <c r="F34" s="340"/>
+      <c r="G34" s="352"/>
       <c r="H34" s="12">
         <f t="shared" ref="H34:H39" si="8">($D$43/8/2)*2+(H33)</f>
         <v>61.25</v>
@@ -43377,12 +43377,12 @@
       </c>
     </row>
     <row r="35" spans="2:24">
-      <c r="B35" s="333"/>
-      <c r="C35" s="344"/>
-      <c r="D35" s="338"/>
-      <c r="E35" s="338"/>
-      <c r="F35" s="338"/>
-      <c r="G35" s="345"/>
+      <c r="B35" s="346"/>
+      <c r="C35" s="351"/>
+      <c r="D35" s="340"/>
+      <c r="E35" s="340"/>
+      <c r="F35" s="340"/>
+      <c r="G35" s="352"/>
       <c r="H35" s="12">
         <f t="shared" si="8"/>
         <v>73.75</v>
@@ -43397,12 +43397,12 @@
       </c>
     </row>
     <row r="36" spans="2:24">
-      <c r="B36" s="333"/>
-      <c r="C36" s="344"/>
-      <c r="D36" s="338"/>
-      <c r="E36" s="338"/>
-      <c r="F36" s="338"/>
-      <c r="G36" s="345"/>
+      <c r="B36" s="346"/>
+      <c r="C36" s="351"/>
+      <c r="D36" s="340"/>
+      <c r="E36" s="340"/>
+      <c r="F36" s="340"/>
+      <c r="G36" s="352"/>
       <c r="H36" s="12">
         <f t="shared" si="8"/>
         <v>86.25</v>
@@ -43417,12 +43417,12 @@
       </c>
     </row>
     <row r="37" spans="2:24">
-      <c r="B37" s="333"/>
-      <c r="C37" s="344"/>
-      <c r="D37" s="338"/>
-      <c r="E37" s="338"/>
-      <c r="F37" s="338"/>
-      <c r="G37" s="345"/>
+      <c r="B37" s="346"/>
+      <c r="C37" s="351"/>
+      <c r="D37" s="340"/>
+      <c r="E37" s="340"/>
+      <c r="F37" s="340"/>
+      <c r="G37" s="352"/>
       <c r="H37" s="12">
         <f t="shared" si="8"/>
         <v>98.75</v>
@@ -43437,12 +43437,12 @@
       </c>
     </row>
     <row r="38" spans="2:24">
-      <c r="B38" s="333"/>
-      <c r="C38" s="344"/>
-      <c r="D38" s="338"/>
-      <c r="E38" s="338"/>
-      <c r="F38" s="338"/>
-      <c r="G38" s="345"/>
+      <c r="B38" s="346"/>
+      <c r="C38" s="351"/>
+      <c r="D38" s="340"/>
+      <c r="E38" s="340"/>
+      <c r="F38" s="340"/>
+      <c r="G38" s="352"/>
       <c r="H38" s="12">
         <f t="shared" si="8"/>
         <v>111.25</v>
@@ -43457,12 +43457,12 @@
       </c>
     </row>
     <row r="39" spans="2:24" ht="14.45" customHeight="1">
-      <c r="B39" s="333"/>
-      <c r="C39" s="344"/>
-      <c r="D39" s="338"/>
-      <c r="E39" s="338"/>
-      <c r="F39" s="338"/>
-      <c r="G39" s="345"/>
+      <c r="B39" s="346"/>
+      <c r="C39" s="351"/>
+      <c r="D39" s="340"/>
+      <c r="E39" s="340"/>
+      <c r="F39" s="340"/>
+      <c r="G39" s="352"/>
       <c r="H39" s="12">
         <f t="shared" si="8"/>
         <v>123.75</v>
@@ -43477,12 +43477,12 @@
       </c>
     </row>
     <row r="40" spans="2:24" ht="15" thickBot="1">
-      <c r="B40" s="337"/>
-      <c r="C40" s="346"/>
-      <c r="D40" s="347"/>
-      <c r="E40" s="347"/>
-      <c r="F40" s="347"/>
-      <c r="G40" s="348"/>
+      <c r="B40" s="347"/>
+      <c r="C40" s="353"/>
+      <c r="D40" s="354"/>
+      <c r="E40" s="354"/>
+      <c r="F40" s="354"/>
+      <c r="G40" s="355"/>
       <c r="H40" s="12">
         <f>D43+H22</f>
         <v>130</v>
@@ -43497,7 +43497,7 @@
       </c>
     </row>
     <row r="41" spans="2:24" ht="28.5">
-      <c r="B41" s="342" t="s">
+      <c r="B41" s="333" t="s">
         <v>191</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -43506,7 +43506,7 @@
       <c r="H41" s="12"/>
     </row>
     <row r="42" spans="2:24">
-      <c r="B42" s="338"/>
+      <c r="B42" s="340"/>
       <c r="C42" s="1" t="s">
         <v>195</v>
       </c>
@@ -43527,7 +43527,7 @@
       <c r="H42" s="12"/>
     </row>
     <row r="43" spans="2:24" ht="28.9" customHeight="1">
-      <c r="B43" s="338"/>
+      <c r="B43" s="340"/>
       <c r="C43" s="1" t="s">
         <v>205</v>
       </c>
@@ -43549,46 +43549,46 @@
       <c r="B44" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C44" s="338" t="s">
+      <c r="C44" s="340" t="s">
         <v>206</v>
       </c>
-      <c r="D44" s="338"/>
-      <c r="E44" s="338"/>
-      <c r="F44" s="338"/>
-      <c r="G44" s="338"/>
+      <c r="D44" s="340"/>
+      <c r="E44" s="340"/>
+      <c r="F44" s="340"/>
+      <c r="G44" s="340"/>
     </row>
     <row r="45" spans="2:24">
-      <c r="B45" s="338" t="s">
+      <c r="B45" s="340" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="46" spans="2:24">
-      <c r="B46" s="338"/>
+      <c r="B46" s="340"/>
     </row>
     <row r="47" spans="2:24" ht="15" thickBot="1">
-      <c r="B47" s="338"/>
+      <c r="B47" s="340"/>
     </row>
     <row r="48" spans="2:24" ht="15" customHeight="1" thickBot="1">
-      <c r="K48" s="349" t="s">
+      <c r="K48" s="341" t="s">
         <v>207</v>
       </c>
-      <c r="L48" s="351"/>
-      <c r="W48" s="339" t="s">
+      <c r="L48" s="342"/>
+      <c r="W48" s="343" t="s">
         <v>207</v>
       </c>
-      <c r="X48" s="339"/>
+      <c r="X48" s="343"/>
     </row>
     <row r="49" spans="2:24" ht="15" thickBot="1">
       <c r="B49" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C49" s="349" t="s">
+      <c r="C49" s="341" t="s">
         <v>208</v>
       </c>
-      <c r="D49" s="350"/>
-      <c r="E49" s="350"/>
-      <c r="F49" s="350"/>
-      <c r="G49" s="351"/>
+      <c r="D49" s="344"/>
+      <c r="E49" s="344"/>
+      <c r="F49" s="344"/>
+      <c r="G49" s="342"/>
       <c r="H49" s="51" t="s">
         <v>186</v>
       </c>
@@ -43607,13 +43607,13 @@
       <c r="N49" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="O49" s="349" t="s">
+      <c r="O49" s="341" t="s">
         <v>212</v>
       </c>
-      <c r="P49" s="350"/>
-      <c r="Q49" s="350"/>
-      <c r="R49" s="350"/>
-      <c r="S49" s="351"/>
+      <c r="P49" s="344"/>
+      <c r="Q49" s="344"/>
+      <c r="R49" s="344"/>
+      <c r="S49" s="342"/>
       <c r="T49" s="1" t="s">
         <v>186</v>
       </c>
@@ -43631,14 +43631,14 @@
       </c>
     </row>
     <row r="50" spans="2:24">
-      <c r="B50" s="332" t="s">
+      <c r="B50" s="345" t="s">
         <v>214</v>
       </c>
-      <c r="C50" s="330"/>
-      <c r="D50" s="343"/>
-      <c r="E50" s="343"/>
-      <c r="F50" s="343"/>
-      <c r="G50" s="331"/>
+      <c r="C50" s="348"/>
+      <c r="D50" s="349"/>
+      <c r="E50" s="349"/>
+      <c r="F50" s="349"/>
+      <c r="G50" s="350"/>
       <c r="H50" s="86">
         <f>($H$40-D68-D65)</f>
         <v>110</v>
@@ -43659,14 +43659,14 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="N50" s="332" t="s">
+      <c r="N50" s="345" t="s">
         <v>214</v>
       </c>
-      <c r="O50" s="330"/>
-      <c r="P50" s="343"/>
-      <c r="Q50" s="343"/>
-      <c r="R50" s="343"/>
-      <c r="S50" s="331"/>
+      <c r="O50" s="348"/>
+      <c r="P50" s="349"/>
+      <c r="Q50" s="349"/>
+      <c r="R50" s="349"/>
+      <c r="S50" s="350"/>
       <c r="T50" s="12">
         <f>($H$40-P68-P65)</f>
         <v>110</v>
@@ -43685,12 +43685,12 @@
       </c>
     </row>
     <row r="51" spans="2:24">
-      <c r="B51" s="333"/>
-      <c r="C51" s="344"/>
-      <c r="D51" s="338"/>
-      <c r="E51" s="338"/>
-      <c r="F51" s="338"/>
-      <c r="G51" s="345"/>
+      <c r="B51" s="346"/>
+      <c r="C51" s="351"/>
+      <c r="D51" s="340"/>
+      <c r="E51" s="340"/>
+      <c r="F51" s="340"/>
+      <c r="G51" s="352"/>
       <c r="H51" s="86">
         <f>(H58-H50)/8/2+H50</f>
         <v>110.9375</v>
@@ -43710,12 +43710,12 @@
       <c r="L51" s="93">
         <v>3</v>
       </c>
-      <c r="N51" s="333"/>
-      <c r="O51" s="344"/>
-      <c r="P51" s="338"/>
-      <c r="Q51" s="338"/>
-      <c r="R51" s="338"/>
-      <c r="S51" s="345"/>
+      <c r="N51" s="346"/>
+      <c r="O51" s="351"/>
+      <c r="P51" s="340"/>
+      <c r="Q51" s="340"/>
+      <c r="R51" s="340"/>
+      <c r="S51" s="352"/>
       <c r="T51" s="1">
         <f>(T58-T50)/8/2+T50</f>
         <v>110.9375</v>
@@ -43736,12 +43736,12 @@
       </c>
     </row>
     <row r="52" spans="2:24">
-      <c r="B52" s="333"/>
-      <c r="C52" s="344"/>
-      <c r="D52" s="338"/>
-      <c r="E52" s="338"/>
-      <c r="F52" s="338"/>
-      <c r="G52" s="345"/>
+      <c r="B52" s="346"/>
+      <c r="C52" s="351"/>
+      <c r="D52" s="340"/>
+      <c r="E52" s="340"/>
+      <c r="F52" s="340"/>
+      <c r="G52" s="352"/>
       <c r="H52" s="86">
         <f t="shared" ref="H52:H57" si="13">($H$58-$H$50)/8+H51</f>
         <v>112.8125</v>
@@ -43762,12 +43762,12 @@
         <f>I51</f>
         <v>7.75</v>
       </c>
-      <c r="N52" s="333"/>
-      <c r="O52" s="344"/>
-      <c r="P52" s="338"/>
-      <c r="Q52" s="338"/>
-      <c r="R52" s="338"/>
-      <c r="S52" s="345"/>
+      <c r="N52" s="346"/>
+      <c r="O52" s="351"/>
+      <c r="P52" s="340"/>
+      <c r="Q52" s="340"/>
+      <c r="R52" s="340"/>
+      <c r="S52" s="352"/>
       <c r="T52" s="1">
         <f t="shared" ref="T52:T57" si="14">($H$58-$H$50)/8+T51</f>
         <v>112.8125</v>
@@ -43788,12 +43788,12 @@
       </c>
     </row>
     <row r="53" spans="2:24">
-      <c r="B53" s="333"/>
-      <c r="C53" s="344"/>
-      <c r="D53" s="338"/>
-      <c r="E53" s="338"/>
-      <c r="F53" s="338"/>
-      <c r="G53" s="345"/>
+      <c r="B53" s="346"/>
+      <c r="C53" s="351"/>
+      <c r="D53" s="340"/>
+      <c r="E53" s="340"/>
+      <c r="F53" s="340"/>
+      <c r="G53" s="352"/>
       <c r="H53" s="86">
         <f t="shared" si="13"/>
         <v>114.6875</v>
@@ -43814,12 +43814,12 @@
         <f t="shared" ref="L53:L57" si="16">I52</f>
         <v>15.25</v>
       </c>
-      <c r="N53" s="333"/>
-      <c r="O53" s="344"/>
-      <c r="P53" s="338"/>
-      <c r="Q53" s="338"/>
-      <c r="R53" s="338"/>
-      <c r="S53" s="345"/>
+      <c r="N53" s="346"/>
+      <c r="O53" s="351"/>
+      <c r="P53" s="340"/>
+      <c r="Q53" s="340"/>
+      <c r="R53" s="340"/>
+      <c r="S53" s="352"/>
       <c r="T53" s="1">
         <f t="shared" si="14"/>
         <v>114.6875</v>
@@ -43840,12 +43840,12 @@
       </c>
     </row>
     <row r="54" spans="2:24">
-      <c r="B54" s="333"/>
-      <c r="C54" s="344"/>
-      <c r="D54" s="338"/>
-      <c r="E54" s="338"/>
-      <c r="F54" s="338"/>
-      <c r="G54" s="345"/>
+      <c r="B54" s="346"/>
+      <c r="C54" s="351"/>
+      <c r="D54" s="340"/>
+      <c r="E54" s="340"/>
+      <c r="F54" s="340"/>
+      <c r="G54" s="352"/>
       <c r="H54" s="86">
         <f t="shared" si="13"/>
         <v>116.5625</v>
@@ -43866,12 +43866,12 @@
         <f t="shared" si="16"/>
         <v>22.75</v>
       </c>
-      <c r="N54" s="333"/>
-      <c r="O54" s="344"/>
-      <c r="P54" s="338"/>
-      <c r="Q54" s="338"/>
-      <c r="R54" s="338"/>
-      <c r="S54" s="345"/>
+      <c r="N54" s="346"/>
+      <c r="O54" s="351"/>
+      <c r="P54" s="340"/>
+      <c r="Q54" s="340"/>
+      <c r="R54" s="340"/>
+      <c r="S54" s="352"/>
       <c r="T54" s="1">
         <f t="shared" si="14"/>
         <v>116.5625</v>
@@ -43892,12 +43892,12 @@
       </c>
     </row>
     <row r="55" spans="2:24">
-      <c r="B55" s="333"/>
-      <c r="C55" s="344"/>
-      <c r="D55" s="338"/>
-      <c r="E55" s="338"/>
-      <c r="F55" s="338"/>
-      <c r="G55" s="345"/>
+      <c r="B55" s="346"/>
+      <c r="C55" s="351"/>
+      <c r="D55" s="340"/>
+      <c r="E55" s="340"/>
+      <c r="F55" s="340"/>
+      <c r="G55" s="352"/>
       <c r="H55" s="86">
         <f t="shared" si="13"/>
         <v>118.4375</v>
@@ -43918,12 +43918,12 @@
         <f t="shared" si="16"/>
         <v>24</v>
       </c>
-      <c r="N55" s="333"/>
-      <c r="O55" s="344"/>
-      <c r="P55" s="338"/>
-      <c r="Q55" s="338"/>
-      <c r="R55" s="338"/>
-      <c r="S55" s="345"/>
+      <c r="N55" s="346"/>
+      <c r="O55" s="351"/>
+      <c r="P55" s="340"/>
+      <c r="Q55" s="340"/>
+      <c r="R55" s="340"/>
+      <c r="S55" s="352"/>
       <c r="T55" s="1">
         <f t="shared" si="14"/>
         <v>118.4375</v>
@@ -43944,12 +43944,12 @@
       </c>
     </row>
     <row r="56" spans="2:24">
-      <c r="B56" s="333"/>
-      <c r="C56" s="344"/>
-      <c r="D56" s="338"/>
-      <c r="E56" s="338"/>
-      <c r="F56" s="338"/>
-      <c r="G56" s="345"/>
+      <c r="B56" s="346"/>
+      <c r="C56" s="351"/>
+      <c r="D56" s="340"/>
+      <c r="E56" s="340"/>
+      <c r="F56" s="340"/>
+      <c r="G56" s="352"/>
       <c r="H56" s="86">
         <f t="shared" si="13"/>
         <v>120.3125</v>
@@ -43970,12 +43970,12 @@
         <f t="shared" si="16"/>
         <v>24</v>
       </c>
-      <c r="N56" s="333"/>
-      <c r="O56" s="344"/>
-      <c r="P56" s="338"/>
-      <c r="Q56" s="338"/>
-      <c r="R56" s="338"/>
-      <c r="S56" s="345"/>
+      <c r="N56" s="346"/>
+      <c r="O56" s="351"/>
+      <c r="P56" s="340"/>
+      <c r="Q56" s="340"/>
+      <c r="R56" s="340"/>
+      <c r="S56" s="352"/>
       <c r="T56" s="1">
         <f t="shared" si="14"/>
         <v>120.3125</v>
@@ -43996,12 +43996,12 @@
       </c>
     </row>
     <row r="57" spans="2:24">
-      <c r="B57" s="333"/>
-      <c r="C57" s="344"/>
-      <c r="D57" s="338"/>
-      <c r="E57" s="338"/>
-      <c r="F57" s="338"/>
-      <c r="G57" s="345"/>
+      <c r="B57" s="346"/>
+      <c r="C57" s="351"/>
+      <c r="D57" s="340"/>
+      <c r="E57" s="340"/>
+      <c r="F57" s="340"/>
+      <c r="G57" s="352"/>
       <c r="H57" s="86">
         <f t="shared" si="13"/>
         <v>122.1875</v>
@@ -44022,12 +44022,12 @@
         <f t="shared" si="16"/>
         <v>24</v>
       </c>
-      <c r="N57" s="333"/>
-      <c r="O57" s="344"/>
-      <c r="P57" s="338"/>
-      <c r="Q57" s="338"/>
-      <c r="R57" s="338"/>
-      <c r="S57" s="345"/>
+      <c r="N57" s="346"/>
+      <c r="O57" s="351"/>
+      <c r="P57" s="340"/>
+      <c r="Q57" s="340"/>
+      <c r="R57" s="340"/>
+      <c r="S57" s="352"/>
       <c r="T57" s="1">
         <f t="shared" si="14"/>
         <v>122.1875</v>
@@ -44048,12 +44048,12 @@
       </c>
     </row>
     <row r="58" spans="2:24">
-      <c r="B58" s="333"/>
-      <c r="C58" s="344"/>
-      <c r="D58" s="338"/>
-      <c r="E58" s="338"/>
-      <c r="F58" s="338"/>
-      <c r="G58" s="345"/>
+      <c r="B58" s="346"/>
+      <c r="C58" s="351"/>
+      <c r="D58" s="340"/>
+      <c r="E58" s="340"/>
+      <c r="F58" s="340"/>
+      <c r="G58" s="352"/>
       <c r="H58" s="86">
         <f>$H$50+D65</f>
         <v>125</v>
@@ -44074,12 +44074,12 @@
         <f>IF(((($D$67)/($D$65-$D$64))*(K58-$H$50)+$I$40)&gt;($D$67+$I$40),($D$67+$I$40),(($D$67)/($D$65-$D$64))*(K58-$H$50)+$I$40)</f>
         <v>24</v>
       </c>
-      <c r="N58" s="333"/>
-      <c r="O58" s="344"/>
-      <c r="P58" s="338"/>
-      <c r="Q58" s="338"/>
-      <c r="R58" s="338"/>
-      <c r="S58" s="345"/>
+      <c r="N58" s="346"/>
+      <c r="O58" s="351"/>
+      <c r="P58" s="340"/>
+      <c r="Q58" s="340"/>
+      <c r="R58" s="340"/>
+      <c r="S58" s="352"/>
       <c r="T58" s="12">
         <f>$H$50+P65</f>
         <v>125</v>
@@ -44100,12 +44100,12 @@
       </c>
     </row>
     <row r="59" spans="2:24" ht="15" customHeight="1" thickBot="1">
-      <c r="B59" s="337"/>
-      <c r="C59" s="352"/>
-      <c r="D59" s="353"/>
-      <c r="E59" s="353"/>
-      <c r="F59" s="353"/>
-      <c r="G59" s="354"/>
+      <c r="B59" s="347"/>
+      <c r="C59" s="356"/>
+      <c r="D59" s="357"/>
+      <c r="E59" s="357"/>
+      <c r="F59" s="357"/>
+      <c r="G59" s="358"/>
       <c r="H59" s="89">
         <f>H58</f>
         <v>125</v>
@@ -44126,12 +44126,12 @@
         <f>L50</f>
         <v>0</v>
       </c>
-      <c r="N59" s="337"/>
-      <c r="O59" s="346"/>
-      <c r="P59" s="347"/>
-      <c r="Q59" s="347"/>
-      <c r="R59" s="347"/>
-      <c r="S59" s="348"/>
+      <c r="N59" s="347"/>
+      <c r="O59" s="353"/>
+      <c r="P59" s="354"/>
+      <c r="Q59" s="354"/>
+      <c r="R59" s="354"/>
+      <c r="S59" s="355"/>
       <c r="T59" s="12">
         <f>T58</f>
         <v>125</v>
@@ -44146,7 +44146,7 @@
       </c>
     </row>
     <row r="60" spans="2:24" ht="16.149999999999999" customHeight="1">
-      <c r="B60" s="355" t="s">
+      <c r="B60" s="359" t="s">
         <v>191</v>
       </c>
       <c r="C60" s="82" t="s">
@@ -44166,11 +44166,11 @@
       <c r="G60" s="57" t="s">
         <v>217</v>
       </c>
-      <c r="H60" s="360" t="s">
+      <c r="H60" s="334" t="s">
         <v>218</v>
       </c>
-      <c r="I60" s="361"/>
-      <c r="J60" s="362"/>
+      <c r="I60" s="335"/>
+      <c r="J60" s="336"/>
       <c r="K60" s="82" t="s">
         <v>219</v>
       </c>
@@ -44178,7 +44178,7 @@
         <f>K67^2/K68</f>
         <v>1.1707317073170729</v>
       </c>
-      <c r="N60" s="342" t="s">
+      <c r="N60" s="333" t="s">
         <v>191</v>
       </c>
       <c r="O60" s="1" t="s">
@@ -44186,7 +44186,7 @@
       </c>
     </row>
     <row r="61" spans="2:24" ht="16.149999999999999" customHeight="1" thickBot="1">
-      <c r="B61" s="356"/>
+      <c r="B61" s="360"/>
       <c r="C61" s="81" t="s">
         <v>221</v>
       </c>
@@ -44197,15 +44197,15 @@
       <c r="E61" s="78"/>
       <c r="F61" s="61"/>
       <c r="G61" s="62"/>
-      <c r="H61" s="363"/>
-      <c r="I61" s="364"/>
-      <c r="J61" s="365"/>
+      <c r="H61" s="337"/>
+      <c r="I61" s="338"/>
+      <c r="J61" s="339"/>
       <c r="K61" s="81"/>
       <c r="L61" s="62"/>
-      <c r="N61" s="342"/>
+      <c r="N61" s="333"/>
     </row>
     <row r="62" spans="2:24" ht="27.6" customHeight="1">
-      <c r="B62" s="356"/>
+      <c r="B62" s="360"/>
       <c r="C62" s="80" t="s">
         <v>222</v>
       </c>
@@ -44223,10 +44223,10 @@
         <v>225</v>
       </c>
       <c r="L62" s="59"/>
-      <c r="N62" s="342"/>
+      <c r="N62" s="333"/>
     </row>
     <row r="63" spans="2:24" ht="27.6" customHeight="1">
-      <c r="B63" s="356"/>
+      <c r="B63" s="360"/>
       <c r="C63" s="80" t="s">
         <v>226</v>
       </c>
@@ -44243,10 +44243,10 @@
         <v>15</v>
       </c>
       <c r="L63" s="59"/>
-      <c r="N63" s="342"/>
+      <c r="N63" s="333"/>
     </row>
     <row r="64" spans="2:24">
-      <c r="B64" s="357"/>
+      <c r="B64" s="361"/>
       <c r="C64" s="77" t="s">
         <v>229</v>
       </c>
@@ -44281,7 +44281,7 @@
       <c r="L64" s="59" t="s">
         <v>197</v>
       </c>
-      <c r="N64" s="342"/>
+      <c r="N64" s="333"/>
       <c r="O64" s="1" t="s">
         <v>229</v>
       </c>
@@ -44301,7 +44301,7 @@
       </c>
     </row>
     <row r="65" spans="2:19">
-      <c r="B65" s="358"/>
+      <c r="B65" s="362"/>
       <c r="C65" s="77" t="s">
         <v>230</v>
       </c>
@@ -44336,7 +44336,7 @@
       <c r="L65" s="59" t="s">
         <v>197</v>
       </c>
-      <c r="N65" s="338"/>
+      <c r="N65" s="340"/>
       <c r="O65" s="1" t="s">
         <v>230</v>
       </c>
@@ -44356,7 +44356,7 @@
       </c>
     </row>
     <row r="66" spans="2:19">
-      <c r="B66" s="358"/>
+      <c r="B66" s="362"/>
       <c r="C66" s="77" t="s">
         <v>231</v>
       </c>
@@ -44382,10 +44382,10 @@
         <v>0.32258064516129015</v>
       </c>
       <c r="L66" s="59"/>
-      <c r="N66" s="338"/>
+      <c r="N66" s="340"/>
     </row>
     <row r="67" spans="2:19">
-      <c r="B67" s="358"/>
+      <c r="B67" s="362"/>
       <c r="C67" s="77" t="s">
         <v>232</v>
       </c>
@@ -44420,7 +44420,7 @@
       <c r="L67" s="59" t="s">
         <v>197</v>
       </c>
-      <c r="N67" s="338"/>
+      <c r="N67" s="340"/>
       <c r="O67" s="1" t="s">
         <v>232</v>
       </c>
@@ -44440,7 +44440,7 @@
       </c>
     </row>
     <row r="68" spans="2:19" ht="29.25" thickBot="1">
-      <c r="B68" s="359"/>
+      <c r="B68" s="363"/>
       <c r="C68" s="78" t="s">
         <v>234</v>
       </c>
@@ -44474,7 +44474,7 @@
       <c r="L68" s="62" t="s">
         <v>223</v>
       </c>
-      <c r="N68" s="338"/>
+      <c r="N68" s="340"/>
       <c r="O68" s="1" t="s">
         <v>234</v>
       </c>
@@ -44496,26 +44496,26 @@
       <c r="B69" s="55" t="s">
         <v>199</v>
       </c>
-      <c r="C69" s="342" t="s">
+      <c r="C69" s="333" t="s">
         <v>237</v>
       </c>
-      <c r="D69" s="342"/>
-      <c r="E69" s="342"/>
-      <c r="F69" s="342"/>
-      <c r="G69" s="342"/>
+      <c r="D69" s="333"/>
+      <c r="E69" s="333"/>
+      <c r="F69" s="333"/>
+      <c r="G69" s="333"/>
       <c r="N69" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="O69" s="338" t="s">
+      <c r="O69" s="340" t="s">
         <v>238</v>
       </c>
-      <c r="P69" s="338"/>
-      <c r="Q69" s="338"/>
-      <c r="R69" s="338"/>
-      <c r="S69" s="338"/>
+      <c r="P69" s="340"/>
+      <c r="Q69" s="340"/>
+      <c r="R69" s="340"/>
+      <c r="S69" s="340"/>
     </row>
     <row r="70" spans="2:19">
-      <c r="B70" s="338" t="s">
+      <c r="B70" s="340" t="s">
         <v>201</v>
       </c>
       <c r="C70" s="66"/>
@@ -44523,24 +44523,24 @@
       <c r="E70" s="65"/>
       <c r="F70" s="65"/>
       <c r="G70" s="94"/>
-      <c r="N70" s="338" t="s">
+      <c r="N70" s="340" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="71" spans="2:19">
-      <c r="B71" s="338"/>
+      <c r="B71" s="340"/>
       <c r="C71" s="67"/>
       <c r="G71" s="95"/>
-      <c r="N71" s="338"/>
+      <c r="N71" s="340"/>
     </row>
     <row r="72" spans="2:19">
-      <c r="B72" s="338"/>
+      <c r="B72" s="340"/>
       <c r="C72" s="68"/>
       <c r="D72" s="69"/>
       <c r="E72" s="69"/>
       <c r="F72" s="69"/>
       <c r="G72" s="96"/>
-      <c r="N72" s="338"/>
+      <c r="N72" s="340"/>
     </row>
     <row r="73" spans="2:19" ht="15" thickBot="1"/>
     <row r="74" spans="2:19" ht="15" thickBot="1">
@@ -44664,14 +44664,14 @@
       </c>
     </row>
     <row r="88" spans="2:10">
-      <c r="B88" s="332" t="s">
+      <c r="B88" s="345" t="s">
         <v>246</v>
       </c>
-      <c r="C88" s="330"/>
-      <c r="D88" s="343"/>
-      <c r="E88" s="343"/>
-      <c r="F88" s="343"/>
-      <c r="G88" s="331"/>
+      <c r="C88" s="348"/>
+      <c r="D88" s="349"/>
+      <c r="E88" s="349"/>
+      <c r="F88" s="349"/>
+      <c r="G88" s="350"/>
       <c r="H88" s="11">
         <f>H40</f>
         <v>130</v>
@@ -44686,12 +44686,12 @@
       </c>
     </row>
     <row r="89" spans="2:10">
-      <c r="B89" s="333"/>
-      <c r="C89" s="344"/>
-      <c r="D89" s="338"/>
-      <c r="E89" s="338"/>
-      <c r="F89" s="338"/>
-      <c r="G89" s="345"/>
+      <c r="B89" s="346"/>
+      <c r="C89" s="351"/>
+      <c r="D89" s="340"/>
+      <c r="E89" s="340"/>
+      <c r="F89" s="340"/>
+      <c r="G89" s="352"/>
       <c r="H89" s="11">
         <f>($D$100/8/2)+H88</f>
         <v>130.5</v>
@@ -44706,12 +44706,12 @@
       </c>
     </row>
     <row r="90" spans="2:10">
-      <c r="B90" s="333"/>
-      <c r="C90" s="344"/>
-      <c r="D90" s="338"/>
-      <c r="E90" s="338"/>
-      <c r="F90" s="338"/>
-      <c r="G90" s="345"/>
+      <c r="B90" s="346"/>
+      <c r="C90" s="351"/>
+      <c r="D90" s="340"/>
+      <c r="E90" s="340"/>
+      <c r="F90" s="340"/>
+      <c r="G90" s="352"/>
       <c r="H90" s="11">
         <f>($D$100/8)+H89</f>
         <v>131.5</v>
@@ -44726,12 +44726,12 @@
       </c>
     </row>
     <row r="91" spans="2:10">
-      <c r="B91" s="333"/>
-      <c r="C91" s="344"/>
-      <c r="D91" s="338"/>
-      <c r="E91" s="338"/>
-      <c r="F91" s="338"/>
-      <c r="G91" s="345"/>
+      <c r="B91" s="346"/>
+      <c r="C91" s="351"/>
+      <c r="D91" s="340"/>
+      <c r="E91" s="340"/>
+      <c r="F91" s="340"/>
+      <c r="G91" s="352"/>
       <c r="H91" s="11">
         <f t="shared" ref="H91:H96" si="22">($D$100/8)+H90</f>
         <v>132.5</v>
@@ -44746,12 +44746,12 @@
       </c>
     </row>
     <row r="92" spans="2:10">
-      <c r="B92" s="333"/>
-      <c r="C92" s="344"/>
-      <c r="D92" s="338"/>
-      <c r="E92" s="338"/>
-      <c r="F92" s="338"/>
-      <c r="G92" s="345"/>
+      <c r="B92" s="346"/>
+      <c r="C92" s="351"/>
+      <c r="D92" s="340"/>
+      <c r="E92" s="340"/>
+      <c r="F92" s="340"/>
+      <c r="G92" s="352"/>
       <c r="H92" s="11">
         <f t="shared" si="22"/>
         <v>133.5</v>
@@ -44766,12 +44766,12 @@
       </c>
     </row>
     <row r="93" spans="2:10">
-      <c r="B93" s="333"/>
-      <c r="C93" s="344"/>
-      <c r="D93" s="338"/>
-      <c r="E93" s="338"/>
-      <c r="F93" s="338"/>
-      <c r="G93" s="345"/>
+      <c r="B93" s="346"/>
+      <c r="C93" s="351"/>
+      <c r="D93" s="340"/>
+      <c r="E93" s="340"/>
+      <c r="F93" s="340"/>
+      <c r="G93" s="352"/>
       <c r="H93" s="11">
         <f t="shared" si="22"/>
         <v>134.5</v>
@@ -44786,12 +44786,12 @@
       </c>
     </row>
     <row r="94" spans="2:10">
-      <c r="B94" s="333"/>
-      <c r="C94" s="344"/>
-      <c r="D94" s="338"/>
-      <c r="E94" s="338"/>
-      <c r="F94" s="338"/>
-      <c r="G94" s="345"/>
+      <c r="B94" s="346"/>
+      <c r="C94" s="351"/>
+      <c r="D94" s="340"/>
+      <c r="E94" s="340"/>
+      <c r="F94" s="340"/>
+      <c r="G94" s="352"/>
       <c r="H94" s="11">
         <f t="shared" si="22"/>
         <v>135.5</v>
@@ -44806,12 +44806,12 @@
       </c>
     </row>
     <row r="95" spans="2:10">
-      <c r="B95" s="333"/>
-      <c r="C95" s="344"/>
-      <c r="D95" s="338"/>
-      <c r="E95" s="338"/>
-      <c r="F95" s="338"/>
-      <c r="G95" s="345"/>
+      <c r="B95" s="346"/>
+      <c r="C95" s="351"/>
+      <c r="D95" s="340"/>
+      <c r="E95" s="340"/>
+      <c r="F95" s="340"/>
+      <c r="G95" s="352"/>
       <c r="H95" s="11">
         <f t="shared" si="22"/>
         <v>136.5</v>
@@ -44826,12 +44826,12 @@
       </c>
     </row>
     <row r="96" spans="2:10">
-      <c r="B96" s="333"/>
-      <c r="C96" s="344"/>
-      <c r="D96" s="338"/>
-      <c r="E96" s="338"/>
-      <c r="F96" s="338"/>
-      <c r="G96" s="345"/>
+      <c r="B96" s="346"/>
+      <c r="C96" s="351"/>
+      <c r="D96" s="340"/>
+      <c r="E96" s="340"/>
+      <c r="F96" s="340"/>
+      <c r="G96" s="352"/>
       <c r="H96" s="11">
         <f t="shared" si="22"/>
         <v>137.5</v>
@@ -44846,12 +44846,12 @@
       </c>
     </row>
     <row r="97" spans="2:10" ht="15" thickBot="1">
-      <c r="B97" s="337"/>
-      <c r="C97" s="346"/>
-      <c r="D97" s="347"/>
-      <c r="E97" s="347"/>
-      <c r="F97" s="347"/>
-      <c r="G97" s="348"/>
+      <c r="B97" s="347"/>
+      <c r="C97" s="353"/>
+      <c r="D97" s="354"/>
+      <c r="E97" s="354"/>
+      <c r="F97" s="354"/>
+      <c r="G97" s="355"/>
       <c r="H97" s="11">
         <f>D100+H88</f>
         <v>138</v>
@@ -44866,7 +44866,7 @@
       </c>
     </row>
     <row r="98" spans="2:10" ht="28.5">
-      <c r="B98" s="342" t="s">
+      <c r="B98" s="333" t="s">
         <v>191</v>
       </c>
       <c r="C98" s="1" t="s">
@@ -44889,7 +44889,7 @@
       </c>
     </row>
     <row r="99" spans="2:10" ht="28.5">
-      <c r="B99" s="338"/>
+      <c r="B99" s="340"/>
       <c r="C99" s="1" t="s">
         <v>248</v>
       </c>
@@ -44909,7 +44909,7 @@
       </c>
     </row>
     <row r="100" spans="2:10">
-      <c r="B100" s="338"/>
+      <c r="B100" s="340"/>
       <c r="C100" s="1" t="s">
         <v>205</v>
       </c>
@@ -44931,49 +44931,27 @@
       <c r="B101" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="C101" s="338" t="s">
+      <c r="C101" s="340" t="s">
         <v>249</v>
       </c>
-      <c r="D101" s="338"/>
-      <c r="E101" s="338"/>
-      <c r="F101" s="338"/>
-      <c r="G101" s="338"/>
+      <c r="D101" s="340"/>
+      <c r="E101" s="340"/>
+      <c r="F101" s="340"/>
+      <c r="G101" s="340"/>
     </row>
     <row r="102" spans="2:10">
-      <c r="B102" s="338" t="s">
+      <c r="B102" s="340" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="103" spans="2:10">
-      <c r="B103" s="338"/>
+      <c r="B103" s="340"/>
     </row>
     <row r="104" spans="2:10">
-      <c r="B104" s="338"/>
+      <c r="B104" s="340"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="O12:S12"/>
-    <mergeCell ref="O27:S27"/>
-    <mergeCell ref="H60:J61"/>
-    <mergeCell ref="N70:N72"/>
-    <mergeCell ref="O69:S69"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="W48:X48"/>
-    <mergeCell ref="O49:S49"/>
-    <mergeCell ref="N50:N59"/>
-    <mergeCell ref="O50:S59"/>
-    <mergeCell ref="N60:N68"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="B102:B104"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="B50:B59"/>
-    <mergeCell ref="C50:G59"/>
-    <mergeCell ref="B60:B68"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="B88:B97"/>
-    <mergeCell ref="C88:G97"/>
-    <mergeCell ref="B98:B100"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B13:B22"/>
     <mergeCell ref="C12:G12"/>
@@ -44987,6 +44965,28 @@
     <mergeCell ref="B31:B40"/>
     <mergeCell ref="C31:G40"/>
     <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="B102:B104"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="B50:B59"/>
+    <mergeCell ref="C50:G59"/>
+    <mergeCell ref="B60:B68"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="B88:B97"/>
+    <mergeCell ref="C88:G97"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="W48:X48"/>
+    <mergeCell ref="O49:S49"/>
+    <mergeCell ref="N50:N59"/>
+    <mergeCell ref="O50:S59"/>
+    <mergeCell ref="N60:N68"/>
+    <mergeCell ref="O12:S12"/>
+    <mergeCell ref="O27:S27"/>
+    <mergeCell ref="H60:J61"/>
+    <mergeCell ref="N70:N72"/>
+    <mergeCell ref="O69:S69"/>
+    <mergeCell ref="K48:L48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C28" r:id="rId1" display="https://www.youtube.com/watch?v=-05AlwGI7Jo"/>
@@ -55776,8 +55776,8 @@
   <dimension ref="A1:L263"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J51" sqref="J51"/>
+      <pane ySplit="11" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
@@ -60164,26 +60164,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<scriptIds xmlns="http://schemas.microsoft.com/office/extensibility/maker/v1.0" id="script-ids-node-id">
+  <scriptId id="ms-officescript%3A%2F%2Fonedrive_business_itemlink%2F01TZZHJOP2CWSL3XUZNNHKHVGU4KCQQGAX:ms-officescript%3A%2F%2Fonedrive_business_sharinglink%2Fu!aHR0cHM6Ly91YW5sZWR1LW15LnNoYXJlcG9pbnQuY29tLzp1Oi9nL3BlcnNvbmFsL2p1YW5fdmFsYWRlem9fdWFubF9lZHVfbXgvRWZvVnBMM2VtV3RPbzlUVTRvVUlHQmNCRlJyQnlnX2V0OW1LWVd3VTNFU3NaUQ"/>
+</scriptIds>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d7929c02-2ff7-4e2f-b3f4-5d7437463a37" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f5cf7016-d570-4e66-bed5-9c66354e4d60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006416C8A108E61840AFB84A4598B73E55" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b1d8d0092a91b491fa162699921cd7b6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f5cf7016-d570-4e66-bed5-9c66354e4d60" xmlns:ns3="d7929c02-2ff7-4e2f-b3f4-5d7437463a37" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dc769dae83c42ca581dc5110a4ef7ce3" ns2:_="" ns3:_="">
     <xsd:import namespace="f5cf7016-d570-4e66-bed5-9c66354e4d60"/>
@@ -60390,38 +60376,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d7929c02-2ff7-4e2f-b3f4-5d7437463a37" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f5cf7016-d570-4e66-bed5-9c66354e4d60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<scriptIds xmlns="http://schemas.microsoft.com/office/extensibility/maker/v1.0" id="script-ids-node-id">
-  <scriptId id="ms-officescript%3A%2F%2Fonedrive_business_itemlink%2F01TZZHJOP2CWSL3XUZNNHKHVGU4KCQQGAX:ms-officescript%3A%2F%2Fonedrive_business_sharinglink%2Fu!aHR0cHM6Ly91YW5sZWR1LW15LnNoYXJlcG9pbnQuY29tLzp1Oi9nL3BlcnNvbmFsL2p1YW5fdmFsYWRlem9fdWFubF9lZHVfbXgvRWZvVnBMM2VtV3RPbzlUVTRvVUlHQmNCRlJyQnlnX2V0OW1LWVd3VTNFU3NaUQ"/>
-</scriptIds>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D345C14D-6BDC-44A0-B15C-89E893AF066E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE15861E-CBEF-4CC0-85FE-9F52CCE55DFF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/extensibility/maker/v1.0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E42FDC09-86A2-4A8D-9C5A-BD852817852F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d7929c02-2ff7-4e2f-b3f4-5d7437463a37"/>
-    <ds:schemaRef ds:uri="f5cf7016-d570-4e66-bed5-9c66354e4d60"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BA7C14-35B6-43AC-B57B-4A5107295D21}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -60440,10 +60423,27 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E42FDC09-86A2-4A8D-9C5A-BD852817852F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d7929c02-2ff7-4e2f-b3f4-5d7437463a37"/>
+    <ds:schemaRef ds:uri="f5cf7016-d570-4e66-bed5-9c66354e4d60"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE15861E-CBEF-4CC0-85FE-9F52CCE55DFF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D345C14D-6BDC-44A0-B15C-89E893AF066E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/extensibility/maker/v1.0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>